<commit_message>
recoded laborLand score based on fa5 results (and re-ran all following code). also began the process of recoding new themes onto the questions but didn't finish. added two inversion questions to the recode file but haven't re-run the script
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/calibfun@55 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/survey/doc/StateQuestions5.xlsx
+++ b/survey/doc/StateQuestions5.xlsx
@@ -21,202 +21,176 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="183">
   <si>
-    <t>My midwife gave me her full presence</t>
-  </si>
-  <si>
-    <t>P070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INV - I felt pressured to hurry up and push the baby out </t>
-  </si>
-  <si>
-    <t>P071</t>
-  </si>
-  <si>
-    <t>I concentrated fully on my contractions</t>
-  </si>
-  <si>
-    <t>P072</t>
-  </si>
-  <si>
-    <t>I could not speak during contractions</t>
-  </si>
-  <si>
-    <t>P073</t>
-  </si>
-  <si>
-    <t>I could not speak between contractions</t>
-  </si>
-  <si>
-    <t>P074</t>
-  </si>
-  <si>
-    <t>INV - I "lost spirit" at some point during the labor</t>
-  </si>
-  <si>
-    <t>INV*</t>
-  </si>
-  <si>
-    <t>P075</t>
-  </si>
-  <si>
-    <t>My partner and I worked together emotionally</t>
-  </si>
-  <si>
-    <t>P076</t>
-  </si>
-  <si>
-    <t>I felt safe in my surroundings</t>
-  </si>
-  <si>
-    <t>P077</t>
-  </si>
-  <si>
-    <t>INV - I was following someone else‚Äôs timetable for labor</t>
-  </si>
-  <si>
-    <t>P078</t>
-  </si>
-  <si>
-    <t>My partner and I worked together physically</t>
-  </si>
-  <si>
-    <t>P079</t>
-  </si>
-  <si>
-    <t>INV - I approached my labor through conscious reasoning and/or rationality</t>
-  </si>
-  <si>
-    <t>P080</t>
-  </si>
-  <si>
-    <t>INV - I tried to problem solve or think my way through labor</t>
-  </si>
-  <si>
-    <t>laborLand</t>
-  </si>
-  <si>
-    <t>P082</t>
-  </si>
-  <si>
-    <t>I labored primarily with my eyes closed</t>
-  </si>
-  <si>
-    <t>P048</t>
-  </si>
-  <si>
-    <t>The lighting in my labor and birth environment was dimmed, dark, or off</t>
-  </si>
-  <si>
-    <t>unassigned</t>
-  </si>
-  <si>
-    <t>Strongly Disagree | Disagree | Neither Agree nor Disagree | Agree | Strongly Agree</t>
-  </si>
-  <si>
-    <t>P049</t>
-  </si>
-  <si>
-    <t>I labored in a confined space</t>
-  </si>
-  <si>
-    <t>P050</t>
-  </si>
-  <si>
-    <t>I used water to relax and/or relieve pain during my labor</t>
-  </si>
-  <si>
-    <t>Not at All | Very Little | Somewhat | Quite a Bit | A Great Deal</t>
-  </si>
-  <si>
-    <t>physEnv</t>
-  </si>
-  <si>
-    <t>Strongly Agree | Agree | Neither Agree nor Disagree | Disagree | Strongly Disagree</t>
-  </si>
-  <si>
-    <t>P057</t>
-  </si>
-  <si>
-    <t>I vocalized during contractions</t>
-  </si>
-  <si>
-    <t>Never | Almost never | Occasionally | Often | All the time</t>
-  </si>
-  <si>
-    <t>P058</t>
-  </si>
-  <si>
-    <t>During labor, I focused my attention on my breath</t>
-  </si>
-  <si>
-    <t>intensePres</t>
-  </si>
-  <si>
-    <t>P059</t>
-  </si>
-  <si>
-    <t>INV</t>
-  </si>
-  <si>
-    <t>varName</t>
-  </si>
-  <si>
-    <t>varDesc</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Inverted</t>
-  </si>
-  <si>
-    <t>Response Type</t>
-  </si>
-  <si>
-    <t>INV - I was following directions for what to do</t>
-  </si>
-  <si>
-    <t>P132</t>
-  </si>
-  <si>
-    <t>I was in my own little world</t>
-  </si>
-  <si>
-    <t>P135</t>
-  </si>
-  <si>
-    <t>INV - I was acutely aware of how long my labor was taking</t>
-  </si>
-  <si>
-    <t>P136</t>
-  </si>
-  <si>
-    <t>P083</t>
-  </si>
-  <si>
-    <t>My surroundings were calm and comfortable</t>
-  </si>
-  <si>
-    <t>P085</t>
-  </si>
-  <si>
-    <t>P086</t>
-  </si>
-  <si>
-    <t>My behavior was intuitive rather than rational</t>
-  </si>
-  <si>
-    <t>P087</t>
-  </si>
-  <si>
-    <t>I felt uninhibited</t>
-  </si>
-  <si>
-    <t>intuitMov</t>
-  </si>
-  <si>
-    <t>P089</t>
+    <t>MR5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR3*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR4*</t>
+  </si>
+  <si>
+    <t>Everyone at my birth was following my lead</t>
+  </si>
+  <si>
+    <t>P137</t>
+  </si>
+  <si>
+    <t>My external environment felt distant to me</t>
+  </si>
+  <si>
+    <t>P138</t>
+  </si>
+  <si>
+    <t>I felt connected to all the women who have labored and birthed before me</t>
+  </si>
+  <si>
+    <t>P139</t>
+  </si>
+  <si>
+    <t>INV - I found it very difficult to remain relaxed</t>
+  </si>
+  <si>
+    <t>P141</t>
+  </si>
+  <si>
+    <t>I felt a sense of oneness with the world</t>
+  </si>
+  <si>
+    <t>P143</t>
+  </si>
+  <si>
+    <t>I lost track of time</t>
+  </si>
+  <si>
+    <t>P144</t>
+  </si>
+  <si>
+    <t>Time seemed to slow down or stand still</t>
+  </si>
+  <si>
+    <t>P146</t>
+  </si>
+  <si>
+    <t>I was oblivious to the world beyond my immediate environment</t>
+  </si>
+  <si>
+    <t>P147</t>
+  </si>
+  <si>
+    <t>My actions were purposeful and essential, not frantic or excessive</t>
+  </si>
+  <si>
+    <t>INV - People talked too much</t>
+  </si>
+  <si>
+    <t>P111</t>
+  </si>
+  <si>
+    <t>INV - I needed to impress someone</t>
+  </si>
+  <si>
+    <t>P112</t>
+  </si>
+  <si>
+    <t>I moved around the room</t>
+  </si>
+  <si>
+    <t>P113</t>
+  </si>
+  <si>
+    <t>I was relaxed</t>
+  </si>
+  <si>
+    <t>P114</t>
+  </si>
+  <si>
+    <t>INV - I let myself down</t>
+  </si>
+  <si>
+    <t>P115</t>
+  </si>
+  <si>
+    <t>I moved around based on my intuitive knowledge of how to birth</t>
+  </si>
+  <si>
+    <t>P116</t>
+  </si>
+  <si>
+    <t>P117</t>
+  </si>
+  <si>
+    <t>INV - My emotions became overwhelming</t>
+  </si>
+  <si>
+    <t>P118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My birth was a private event </t>
+  </si>
+  <si>
+    <t>P119</t>
+  </si>
+  <si>
+    <t>INV - I struggled to find a steady rhythm</t>
+  </si>
+  <si>
+    <t>P120</t>
+  </si>
+  <si>
+    <t>I gave it "my all" in every moment</t>
+  </si>
+  <si>
+    <t>P121</t>
+  </si>
+  <si>
+    <t>INV - I tried to escape the sensations in my body</t>
+  </si>
+  <si>
+    <t>P123</t>
+  </si>
+  <si>
+    <t>My partner and I seemed to be the only ones in the room</t>
+  </si>
+  <si>
+    <t>fluidReal</t>
+  </si>
+  <si>
+    <t>P126</t>
+  </si>
+  <si>
+    <t>INV - Time was an important factor in my labor (timing contractions, timing in between contractions, timing overall labor duration, etc.)</t>
+  </si>
+  <si>
+    <t>P127</t>
+  </si>
+  <si>
+    <t>INV - I needed to be coached to give birth successfully</t>
+  </si>
+  <si>
+    <t>P130</t>
   </si>
   <si>
     <t>I relinquished rational control of myself and listened to my body</t>
@@ -413,182 +387,214 @@
     <t>MR4</t>
   </si>
   <si>
-    <t>MR5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR3*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR4*</t>
-  </si>
-  <si>
-    <t>Everyone at my birth was following my lead</t>
-  </si>
-  <si>
-    <t>P137</t>
-  </si>
-  <si>
-    <t>My external environment felt distant to me</t>
-  </si>
-  <si>
-    <t>P138</t>
-  </si>
-  <si>
-    <t>I felt connected to all the women who have labored and birthed before me</t>
-  </si>
-  <si>
-    <t>P139</t>
-  </si>
-  <si>
-    <t>INV - I found it very difficult to remain relaxed</t>
-  </si>
-  <si>
-    <t>P141</t>
-  </si>
-  <si>
-    <t>I felt a sense of oneness with the world</t>
-  </si>
-  <si>
-    <t>P143</t>
-  </si>
-  <si>
-    <t>I lost track of time</t>
-  </si>
-  <si>
-    <t>P144</t>
-  </si>
-  <si>
-    <t>Time seemed to slow down or stand still</t>
-  </si>
-  <si>
-    <t>P146</t>
-  </si>
-  <si>
-    <t>I was oblivious to the world beyond my immediate environment</t>
-  </si>
-  <si>
-    <t>P147</t>
-  </si>
-  <si>
-    <t>My actions were purposeful and essential, not frantic or excessive</t>
-  </si>
-  <si>
-    <t>INV - People talked too much</t>
-  </si>
-  <si>
-    <t>P111</t>
-  </si>
-  <si>
-    <t>INV - I needed to impress someone</t>
-  </si>
-  <si>
-    <t>P112</t>
-  </si>
-  <si>
-    <t>I moved around the room</t>
-  </si>
-  <si>
-    <t>P113</t>
-  </si>
-  <si>
-    <t>I was relaxed</t>
-  </si>
-  <si>
-    <t>P114</t>
-  </si>
-  <si>
-    <t>INV - I let myself down</t>
-  </si>
-  <si>
-    <t>P115</t>
-  </si>
-  <si>
-    <t>I moved around based on my intuitive knowledge of how to birth</t>
-  </si>
-  <si>
-    <t>P116</t>
-  </si>
-  <si>
-    <t>P117</t>
-  </si>
-  <si>
-    <t>INV - My emotions became overwhelming</t>
-  </si>
-  <si>
-    <t>P118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My birth was a private event </t>
-  </si>
-  <si>
-    <t>P119</t>
-  </si>
-  <si>
-    <t>INV - I struggled to find a steady rhythm</t>
-  </si>
-  <si>
-    <t>P120</t>
-  </si>
-  <si>
-    <t>I gave it "my all" in every moment</t>
-  </si>
-  <si>
-    <t>P121</t>
-  </si>
-  <si>
-    <t>INV - I tried to escape the sensations in my body</t>
-  </si>
-  <si>
-    <t>P123</t>
-  </si>
-  <si>
-    <t>My partner and I seemed to be the only ones in the room</t>
-  </si>
-  <si>
-    <t>fluidReal</t>
-  </si>
-  <si>
-    <t>P126</t>
-  </si>
-  <si>
-    <t>INV - Time was an important factor in my labor (timing contractions, timing in between contractions, timing overall labor duration, etc.)</t>
-  </si>
-  <si>
-    <t>P127</t>
-  </si>
-  <si>
-    <t>INV - I needed to be coached to give birth successfully</t>
-  </si>
-  <si>
-    <t>P130</t>
+    <t>My midwife gave me her full presence</t>
+  </si>
+  <si>
+    <t>P070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INV - I felt pressured to hurry up and push the baby out </t>
+  </si>
+  <si>
+    <t>P071</t>
+  </si>
+  <si>
+    <t>I concentrated fully on my contractions</t>
+  </si>
+  <si>
+    <t>P072</t>
+  </si>
+  <si>
+    <t>I could not speak during contractions</t>
+  </si>
+  <si>
+    <t>P073</t>
+  </si>
+  <si>
+    <t>I could not speak between contractions</t>
+  </si>
+  <si>
+    <t>P074</t>
+  </si>
+  <si>
+    <t>INV - I "lost spirit" at some point during the labor</t>
+  </si>
+  <si>
+    <t>INV*</t>
+  </si>
+  <si>
+    <t>P075</t>
+  </si>
+  <si>
+    <t>My partner and I worked together emotionally</t>
+  </si>
+  <si>
+    <t>P076</t>
+  </si>
+  <si>
+    <t>I felt safe in my surroundings</t>
+  </si>
+  <si>
+    <t>P077</t>
+  </si>
+  <si>
+    <t>INV - I was following someone else‚Äôs timetable for labor</t>
+  </si>
+  <si>
+    <t>P078</t>
+  </si>
+  <si>
+    <t>My partner and I worked together physically</t>
+  </si>
+  <si>
+    <t>P079</t>
+  </si>
+  <si>
+    <t>INV - I approached my labor through conscious reasoning and/or rationality</t>
+  </si>
+  <si>
+    <t>P080</t>
+  </si>
+  <si>
+    <t>INV - I tried to problem solve or think my way through labor</t>
+  </si>
+  <si>
+    <t>laborLand</t>
+  </si>
+  <si>
+    <t>P082</t>
+  </si>
+  <si>
+    <t>I labored primarily with my eyes closed</t>
+  </si>
+  <si>
+    <t>P048</t>
+  </si>
+  <si>
+    <t>The lighting in my labor and birth environment was dimmed, dark, or off</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>Strongly Disagree | Disagree | Neither Agree nor Disagree | Agree | Strongly Agree</t>
+  </si>
+  <si>
+    <t>P049</t>
+  </si>
+  <si>
+    <t>I labored in a confined space</t>
+  </si>
+  <si>
+    <t>P050</t>
+  </si>
+  <si>
+    <t>I used water to relax and/or relieve pain during my labor</t>
+  </si>
+  <si>
+    <t>Not at All | Very Little | Somewhat | Quite a Bit | A Great Deal</t>
+  </si>
+  <si>
+    <t>physEnv</t>
+  </si>
+  <si>
+    <t>Strongly Agree | Agree | Neither Agree nor Disagree | Disagree | Strongly Disagree</t>
+  </si>
+  <si>
+    <t>P057</t>
+  </si>
+  <si>
+    <t>I vocalized during contractions</t>
+  </si>
+  <si>
+    <t>Never | Almost never | Occasionally | Often | All the time</t>
+  </si>
+  <si>
+    <t>P058</t>
+  </si>
+  <si>
+    <t>During labor, I focused my attention on my breath</t>
+  </si>
+  <si>
+    <t>intensePres</t>
+  </si>
+  <si>
+    <t>P059</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>varName</t>
+  </si>
+  <si>
+    <t>varDesc</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Inverted</t>
+  </si>
+  <si>
+    <t>Response Type</t>
+  </si>
+  <si>
+    <t>INV - I was following directions for what to do</t>
+  </si>
+  <si>
+    <t>P132</t>
+  </si>
+  <si>
+    <t>I was in my own little world</t>
+  </si>
+  <si>
+    <t>P135</t>
+  </si>
+  <si>
+    <t>INV - I was acutely aware of how long my labor was taking</t>
+  </si>
+  <si>
+    <t>P136</t>
+  </si>
+  <si>
+    <t>P083</t>
+  </si>
+  <si>
+    <t>My surroundings were calm and comfortable</t>
+  </si>
+  <si>
+    <t>P085</t>
+  </si>
+  <si>
+    <t>P086</t>
+  </si>
+  <si>
+    <t>My behavior was intuitive rather than rational</t>
+  </si>
+  <si>
+    <t>P087</t>
+  </si>
+  <si>
+    <t>I felt uninhibited</t>
+  </si>
+  <si>
+    <t>intuitMov</t>
+  </si>
+  <si>
+    <t>P089</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -953,7 +959,7 @@
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -964,1368 +970,1369 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
-        <v>112</v>
-      </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C21" t="s">
-        <v>176</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F23" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" t="s">
         <v>181</v>
       </c>
-      <c r="D24" t="s">
-        <v>64</v>
-      </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F24" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>136</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>140</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>176</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>178</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F29" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>35</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="D35" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F35" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="B36" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36" t="s">
-        <v>0</v>
-      </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F36" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
-        <v>135</v>
-      </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F37" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
         <v>132</v>
       </c>
-      <c r="C41" t="s">
-        <v>15</v>
-      </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F41" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F42" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F43" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>179</v>
+        <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="D45" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="F45" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F47" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>144</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F48" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>174</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>175</v>
       </c>
       <c r="D49" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>153</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F51" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="D52" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E52" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F52" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E53" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F53" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>26</v>
+        <v>143</v>
       </c>
       <c r="D54" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F54" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="D55" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F55" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="B56" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E56" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F56" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D59" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F59" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>174</v>
+        <v>46</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="E60" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F60" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D61" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E61" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F61" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D62" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E62" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F62" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B63" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D63" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E63" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F63" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E64" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F64" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" t="s">
+        <v>162</v>
+      </c>
+      <c r="F65" t="s">
         <v>154</v>
-      </c>
-      <c r="B65" t="s">
-        <v>133</v>
-      </c>
-      <c r="C65" t="s">
-        <v>155</v>
-      </c>
-      <c r="D65" t="s">
-        <v>29</v>
-      </c>
-      <c r="E65" t="s">
-        <v>45</v>
-      </c>
-      <c r="F65" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>166</v>
+        <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E66" t="s">
-        <v>45</v>
+        <v>162</v>
       </c>
       <c r="F66" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="D67" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D68" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F68" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>171</v>
+        <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>172</v>
+        <v>44</v>
       </c>
       <c r="D69" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F69" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F70" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="D74" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>44</v>
+        <v>161</v>
       </c>
       <c r="B75" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D75" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F75" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D76" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F76" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D77" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F77" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D78" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F78" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="B79" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
         <v>130</v>
       </c>
-      <c r="C79" t="s">
-        <v>13</v>
-      </c>
       <c r="D79" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F79" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="D80" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F80" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D81" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F81" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B82" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D82" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F82" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="B83" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C83" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="D83" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="F83" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C84" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="D84" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="F84" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F84">
-    <sortCondition ref="D2:D84"/>
+  <sortState ref="A21:F37">
+    <sortCondition ref="A21:A37"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
filling in t-tests & Ms and SDs for results section
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/calibfun@66 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/survey/doc/StateQuestions5.xlsx
+++ b/survey/doc/StateQuestions5.xlsx
@@ -21,199 +21,169 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="181">
   <si>
-    <t>I felt connected to all the women who have labored and birthed before me</t>
-  </si>
-  <si>
-    <t>P139</t>
-  </si>
-  <si>
-    <t>INV - I found it very difficult to remain relaxed</t>
-  </si>
-  <si>
-    <t>P141</t>
-  </si>
-  <si>
-    <t>I felt a sense of oneness with the world</t>
-  </si>
-  <si>
-    <t>P143</t>
-  </si>
-  <si>
-    <t>I lost track of time</t>
-  </si>
-  <si>
-    <t>P144</t>
-  </si>
-  <si>
-    <t>Time seemed to slow down or stand still</t>
-  </si>
-  <si>
-    <t>P146</t>
-  </si>
-  <si>
-    <t>I was oblivious to the world beyond my immediate environment</t>
-  </si>
-  <si>
-    <t>P147</t>
-  </si>
-  <si>
-    <t>My actions were purposeful and essential, not frantic or excessive</t>
-  </si>
-  <si>
-    <t>INV - People talked too much</t>
-  </si>
-  <si>
-    <t>P111</t>
-  </si>
-  <si>
-    <t>INV - I needed to impress someone</t>
-  </si>
-  <si>
-    <t>P112</t>
-  </si>
-  <si>
-    <t>I moved around the room</t>
-  </si>
-  <si>
-    <t>P113</t>
-  </si>
-  <si>
-    <t>I was relaxed</t>
-  </si>
-  <si>
-    <t>P114</t>
-  </si>
-  <si>
-    <t>INV - I let myself down</t>
-  </si>
-  <si>
-    <t>P115</t>
-  </si>
-  <si>
-    <t>I moved around based on my intuitive knowledge of how to birth</t>
-  </si>
-  <si>
-    <t>P116</t>
-  </si>
-  <si>
-    <t>P117</t>
-  </si>
-  <si>
-    <t>INV - My emotions became overwhelming</t>
-  </si>
-  <si>
-    <t>P118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My birth was a private event </t>
-  </si>
-  <si>
-    <t>P119</t>
-  </si>
-  <si>
-    <t>INV - I struggled to find a steady rhythm</t>
-  </si>
-  <si>
-    <t>P120</t>
-  </si>
-  <si>
-    <t>I gave it "my all" in every moment</t>
-  </si>
-  <si>
-    <t>P121</t>
-  </si>
-  <si>
-    <t>INV - I tried to escape the sensations in my body</t>
-  </si>
-  <si>
-    <t>P123</t>
-  </si>
-  <si>
-    <t>My partner and I seemed to be the only ones in the room</t>
-  </si>
-  <si>
-    <t>fluidReal</t>
-  </si>
-  <si>
-    <t>P126</t>
-  </si>
-  <si>
-    <t>INV - Time was an important factor in my labor (timing contractions, timing in between contractions, timing overall labor duration, etc.)</t>
-  </si>
-  <si>
-    <t>P127</t>
-  </si>
-  <si>
-    <t>INV - I needed to be coached to give birth successfully</t>
-  </si>
-  <si>
-    <t>P130</t>
-  </si>
-  <si>
-    <t>I relinquished rational control of myself and listened to my body</t>
-  </si>
-  <si>
-    <t>P090</t>
-  </si>
-  <si>
-    <t>My partner and I felt intimate</t>
-  </si>
-  <si>
-    <t>P092</t>
-  </si>
-  <si>
-    <t>P093</t>
-  </si>
-  <si>
-    <t>I was aware of cues from my body</t>
-  </si>
-  <si>
-    <t>P094</t>
-  </si>
-  <si>
-    <t>I listened to the cues from my body</t>
-  </si>
-  <si>
-    <t>P095</t>
-  </si>
-  <si>
-    <t>I protected by birthing space</t>
-  </si>
-  <si>
-    <t>P096</t>
-  </si>
-  <si>
-    <t>I could not respond to others if they talked or asked me questions</t>
-  </si>
-  <si>
-    <t>P097</t>
-  </si>
-  <si>
-    <t>INV - I let my partner down</t>
-  </si>
-  <si>
-    <t>INV - I felt inhibited in my noises during labor</t>
-  </si>
-  <si>
-    <t>P101</t>
-  </si>
-  <si>
-    <t>My baby and I were partners, working together</t>
-  </si>
-  <si>
-    <t>P102</t>
-  </si>
-  <si>
-    <t>My birthing environment was comfortable and relaxing</t>
-  </si>
-  <si>
-    <t>P103</t>
-  </si>
-  <si>
-    <t>I made spontaneous noises during contractions</t>
-  </si>
-  <si>
-    <t>P104</t>
+    <t>INV - I approached my labor through conscious reasoning and/or rationality</t>
+  </si>
+  <si>
+    <t>P080</t>
+  </si>
+  <si>
+    <t>INV - I tried to problem solve or think my way through labor</t>
+  </si>
+  <si>
+    <t>laborLand</t>
+  </si>
+  <si>
+    <t>P082</t>
+  </si>
+  <si>
+    <t>I labored primarily with my eyes closed</t>
+  </si>
+  <si>
+    <t>P048</t>
+  </si>
+  <si>
+    <t>The lighting in my labor and birth environment was dimmed, dark, or off</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>Strongly Disagree | Disagree | Neither Agree nor Disagree | Agree | Strongly Agree</t>
+  </si>
+  <si>
+    <t>P049</t>
+  </si>
+  <si>
+    <t>I labored in a confined space</t>
+  </si>
+  <si>
+    <t>P050</t>
+  </si>
+  <si>
+    <t>I used water to relax and/or relieve pain during my labor</t>
+  </si>
+  <si>
+    <t>Not at All | Very Little | Somewhat | Quite a Bit | A Great Deal</t>
+  </si>
+  <si>
+    <t>physEnv</t>
+  </si>
+  <si>
+    <t>Strongly Agree | Agree | Neither Agree nor Disagree | Disagree | Strongly Disagree</t>
+  </si>
+  <si>
+    <t>P057</t>
+  </si>
+  <si>
+    <t>I vocalized during contractions</t>
+  </si>
+  <si>
+    <t>Never | Almost never | Occasionally | Often | All the time</t>
+  </si>
+  <si>
+    <t>P058</t>
+  </si>
+  <si>
+    <t>During labor, I focused my attention on my breath</t>
+  </si>
+  <si>
+    <t>intensePres</t>
+  </si>
+  <si>
+    <t>P059</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>varName</t>
+  </si>
+  <si>
+    <t>varDesc</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Inverted</t>
+  </si>
+  <si>
+    <t>Response Type</t>
+  </si>
+  <si>
+    <t>INV - I was following directions for what to do</t>
+  </si>
+  <si>
+    <t>P132</t>
+  </si>
+  <si>
+    <t>I was in my own little world</t>
+  </si>
+  <si>
+    <t>P135</t>
+  </si>
+  <si>
+    <t>INV - I was acutely aware of how long my labor was taking</t>
+  </si>
+  <si>
+    <t>P136</t>
+  </si>
+  <si>
+    <t>P083</t>
+  </si>
+  <si>
+    <t>My surroundings were calm and comfortable</t>
+  </si>
+  <si>
+    <t>P085</t>
+  </si>
+  <si>
+    <t>P086</t>
+  </si>
+  <si>
+    <t>My behavior was intuitive rather than rational</t>
+  </si>
+  <si>
+    <t>P087</t>
+  </si>
+  <si>
+    <t>I felt uninhibited</t>
+  </si>
+  <si>
+    <t>intuitMov</t>
+  </si>
+  <si>
+    <t>P089</t>
+  </si>
+  <si>
+    <t>MR1</t>
+  </si>
+  <si>
+    <t>MR5</t>
+  </si>
+  <si>
+    <t>MR5*</t>
+  </si>
+  <si>
+    <t>MR3</t>
+  </si>
+  <si>
+    <t>MR3*</t>
+  </si>
+  <si>
+    <t>MR2</t>
+  </si>
+  <si>
+    <t>MR2*</t>
+  </si>
+  <si>
+    <t>P098</t>
+  </si>
+  <si>
+    <t>My partner protected my birthing space during labor</t>
+  </si>
+  <si>
+    <t>P099</t>
   </si>
   <si>
     <t>My sense of self dissolved</t>
@@ -405,169 +375,199 @@
     <t>P079</t>
   </si>
   <si>
-    <t>INV - I approached my labor through conscious reasoning and/or rationality</t>
-  </si>
-  <si>
-    <t>P080</t>
-  </si>
-  <si>
-    <t>INV - I tried to problem solve or think my way through labor</t>
-  </si>
-  <si>
-    <t>laborLand</t>
-  </si>
-  <si>
-    <t>P082</t>
-  </si>
-  <si>
-    <t>I labored primarily with my eyes closed</t>
-  </si>
-  <si>
-    <t>P048</t>
-  </si>
-  <si>
-    <t>The lighting in my labor and birth environment was dimmed, dark, or off</t>
-  </si>
-  <si>
-    <t>unassigned</t>
-  </si>
-  <si>
-    <t>Strongly Disagree | Disagree | Neither Agree nor Disagree | Agree | Strongly Agree</t>
-  </si>
-  <si>
-    <t>P049</t>
-  </si>
-  <si>
-    <t>I labored in a confined space</t>
-  </si>
-  <si>
-    <t>P050</t>
-  </si>
-  <si>
-    <t>I used water to relax and/or relieve pain during my labor</t>
-  </si>
-  <si>
-    <t>Not at All | Very Little | Somewhat | Quite a Bit | A Great Deal</t>
-  </si>
-  <si>
-    <t>physEnv</t>
-  </si>
-  <si>
-    <t>Strongly Agree | Agree | Neither Agree nor Disagree | Disagree | Strongly Disagree</t>
-  </si>
-  <si>
-    <t>P057</t>
-  </si>
-  <si>
-    <t>I vocalized during contractions</t>
-  </si>
-  <si>
-    <t>Never | Almost never | Occasionally | Often | All the time</t>
-  </si>
-  <si>
-    <t>P058</t>
-  </si>
-  <si>
-    <t>During labor, I focused my attention on my breath</t>
-  </si>
-  <si>
-    <t>intensePres</t>
-  </si>
-  <si>
-    <t>P059</t>
-  </si>
-  <si>
-    <t>INV</t>
-  </si>
-  <si>
-    <t>varName</t>
-  </si>
-  <si>
-    <t>varDesc</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Inverted</t>
-  </si>
-  <si>
-    <t>Response Type</t>
-  </si>
-  <si>
-    <t>INV - I was following directions for what to do</t>
-  </si>
-  <si>
-    <t>P132</t>
-  </si>
-  <si>
-    <t>I was in my own little world</t>
-  </si>
-  <si>
-    <t>P135</t>
-  </si>
-  <si>
-    <t>INV - I was acutely aware of how long my labor was taking</t>
-  </si>
-  <si>
-    <t>P136</t>
-  </si>
-  <si>
-    <t>P083</t>
-  </si>
-  <si>
-    <t>My surroundings were calm and comfortable</t>
-  </si>
-  <si>
-    <t>P085</t>
-  </si>
-  <si>
-    <t>P086</t>
-  </si>
-  <si>
-    <t>My behavior was intuitive rather than rational</t>
-  </si>
-  <si>
-    <t>P087</t>
-  </si>
-  <si>
-    <t>I felt uninhibited</t>
-  </si>
-  <si>
-    <t>intuitMov</t>
-  </si>
-  <si>
-    <t>P089</t>
-  </si>
-  <si>
-    <t>MR1</t>
-  </si>
-  <si>
-    <t>MR5</t>
-  </si>
-  <si>
-    <t>MR5*</t>
-  </si>
-  <si>
-    <t>MR3</t>
-  </si>
-  <si>
-    <t>MR3*</t>
-  </si>
-  <si>
-    <t>MR2</t>
-  </si>
-  <si>
-    <t>MR2*</t>
-  </si>
-  <si>
-    <t>P098</t>
-  </si>
-  <si>
-    <t>My partner protected my birthing space during labor</t>
-  </si>
-  <si>
-    <t>P099</t>
+    <t>I felt connected to all the women who have labored and birthed before me</t>
+  </si>
+  <si>
+    <t>P139</t>
+  </si>
+  <si>
+    <t>INV - I found it very difficult to remain relaxed</t>
+  </si>
+  <si>
+    <t>P141</t>
+  </si>
+  <si>
+    <t>I felt a sense of oneness with the world</t>
+  </si>
+  <si>
+    <t>P143</t>
+  </si>
+  <si>
+    <t>I lost track of time</t>
+  </si>
+  <si>
+    <t>P144</t>
+  </si>
+  <si>
+    <t>Time seemed to slow down or stand still</t>
+  </si>
+  <si>
+    <t>P146</t>
+  </si>
+  <si>
+    <t>I was oblivious to the world beyond my immediate environment</t>
+  </si>
+  <si>
+    <t>P147</t>
+  </si>
+  <si>
+    <t>My actions were purposeful and essential, not frantic or excessive</t>
+  </si>
+  <si>
+    <t>INV - People talked too much</t>
+  </si>
+  <si>
+    <t>P111</t>
+  </si>
+  <si>
+    <t>INV - I needed to impress someone</t>
+  </si>
+  <si>
+    <t>P112</t>
+  </si>
+  <si>
+    <t>I moved around the room</t>
+  </si>
+  <si>
+    <t>P113</t>
+  </si>
+  <si>
+    <t>I was relaxed</t>
+  </si>
+  <si>
+    <t>P114</t>
+  </si>
+  <si>
+    <t>INV - I let myself down</t>
+  </si>
+  <si>
+    <t>P115</t>
+  </si>
+  <si>
+    <t>I moved around based on my intuitive knowledge of how to birth</t>
+  </si>
+  <si>
+    <t>P116</t>
+  </si>
+  <si>
+    <t>P117</t>
+  </si>
+  <si>
+    <t>INV - My emotions became overwhelming</t>
+  </si>
+  <si>
+    <t>P118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My birth was a private event </t>
+  </si>
+  <si>
+    <t>P119</t>
+  </si>
+  <si>
+    <t>INV - I struggled to find a steady rhythm</t>
+  </si>
+  <si>
+    <t>P120</t>
+  </si>
+  <si>
+    <t>I gave it "my all" in every moment</t>
+  </si>
+  <si>
+    <t>P121</t>
+  </si>
+  <si>
+    <t>INV - I tried to escape the sensations in my body</t>
+  </si>
+  <si>
+    <t>P123</t>
+  </si>
+  <si>
+    <t>My partner and I seemed to be the only ones in the room</t>
+  </si>
+  <si>
+    <t>fluidReal</t>
+  </si>
+  <si>
+    <t>P126</t>
+  </si>
+  <si>
+    <t>INV - Time was an important factor in my labor (timing contractions, timing in between contractions, timing overall labor duration, etc.)</t>
+  </si>
+  <si>
+    <t>P127</t>
+  </si>
+  <si>
+    <t>INV - I needed to be coached to give birth successfully</t>
+  </si>
+  <si>
+    <t>P130</t>
+  </si>
+  <si>
+    <t>I relinquished rational control of myself and listened to my body</t>
+  </si>
+  <si>
+    <t>P090</t>
+  </si>
+  <si>
+    <t>My partner and I felt intimate</t>
+  </si>
+  <si>
+    <t>P092</t>
+  </si>
+  <si>
+    <t>P093</t>
+  </si>
+  <si>
+    <t>I was aware of cues from my body</t>
+  </si>
+  <si>
+    <t>P094</t>
+  </si>
+  <si>
+    <t>I listened to the cues from my body</t>
+  </si>
+  <si>
+    <t>P095</t>
+  </si>
+  <si>
+    <t>I protected by birthing space</t>
+  </si>
+  <si>
+    <t>P096</t>
+  </si>
+  <si>
+    <t>I could not respond to others if they talked or asked me questions</t>
+  </si>
+  <si>
+    <t>P097</t>
+  </si>
+  <si>
+    <t>INV - I let my partner down</t>
+  </si>
+  <si>
+    <t>INV - I felt inhibited in my noises during labor</t>
+  </si>
+  <si>
+    <t>P101</t>
+  </si>
+  <si>
+    <t>My baby and I were partners, working together</t>
+  </si>
+  <si>
+    <t>P102</t>
+  </si>
+  <si>
+    <t>My birthing environment was comfortable and relaxing</t>
+  </si>
+  <si>
+    <t>P103</t>
+  </si>
+  <si>
+    <t>I made spontaneous noises during contractions</t>
+  </si>
+  <si>
+    <t>P104</t>
   </si>
 </sst>
 </file>
@@ -944,7 +944,7 @@
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -955,1360 +955,1360 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>166</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="D28" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F34" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F40" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B44" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F45" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" t="s">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
-        <v>172</v>
-      </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>168</v>
       </c>
       <c r="D49" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F49" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="B50" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>177</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="F50" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="B51" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F52" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="D53" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="F53" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
       <c r="D54" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="F54" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>46</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="F55" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>173</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E56" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F56" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D59" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F59" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>171</v>
       </c>
       <c r="B60" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>56</v>
+        <v>172</v>
       </c>
       <c r="D60" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F60" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>180</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>57</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E61" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C62" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E62" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F62" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="D63" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F64" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="B65" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C65" t="s">
-        <v>26</v>
+        <v>142</v>
       </c>
       <c r="D65" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>33</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="D66" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="E66" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="F66" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D67" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F67" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>180</v>
       </c>
       <c r="B68" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="B69" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="C69" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="D69" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B70" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="C70" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D70" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F70" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C73" t="s">
-        <v>144</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F73" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="B74" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D74" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D75" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F75" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C76" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D76" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F76" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C77" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D77" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F77" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C78" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D78" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C79" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D79" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="B80" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C80" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="D80" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F80" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C81" t="s">
-        <v>179</v>
+        <v>53</v>
       </c>
       <c r="D81" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F81" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>62</v>
+        <v>178</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="C82" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="D82" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B83" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
       <c r="C83" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D83" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="E83" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F83" t="s">
-        <v>142</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
       <c r="B84" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="D84" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="F84" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2318,7 +2318,6 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>